<commit_message>
executed testsuite COOLMATE-005 sucessfully
</commit_message>
<xml_diff>
--- a/Katalon Projects/Test Scenarios/COOLMATE-005.xlsx
+++ b/Katalon Projects/Test Scenarios/COOLMATE-005.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BaoNguyen\OneDrive\Máy tính\Draft Repo On Github\Draft\Katalon Projects\Test Scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EED7EEAA-B3A7-434E-A839-D5984788B138}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCB289F3-4A25-46D5-A7E1-2E0B2832C397}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,16 +20,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -97,7 +87,7 @@
     <t>The address is deleted</t>
   </si>
   <si>
-    <t>TC-003-Delete address</t>
+    <t>TC003-Delete address</t>
   </si>
 </sst>
 </file>
@@ -567,8 +557,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>